<commit_message>
Tesis PISDRSL: Avance a sistema de control
</commit_message>
<xml_diff>
--- a/6_Semestre/Automatizacion_II/Clases/5_PID/Interpolacion.xlsx
+++ b/6_Semestre/Automatizacion_II/Clases/5_PID/Interpolacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Ing_en_automatizacion\6_Semestre\Automatizacion_II\Clases\5_PID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F06A1-7269-4F8F-982C-F3B555DDE1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C57619-CEE7-4B70-9ADB-13647900E24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{717BB28A-F747-4C64-88B9-C1AF063656A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Voltaje</t>
   </si>
@@ -44,16 +44,10 @@
     <t>Luxes</t>
   </si>
   <si>
-    <t>Ohms</t>
+    <t>ADC</t>
   </si>
   <si>
-    <t>Vout</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Vin</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -131,6 +125,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>ADC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -167,23 +186,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Luxes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Luxes</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -194,156 +205,115 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.9331886746228959E-2"/>
+                  <c:y val="0.13086789436444352"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-MX"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Hoja1!$D$3:$D$15</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$C$3:$C$23</c:f>
+              <c:f>Hoja1!$C$3:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>215</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>372</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>470</c:v>
+                  <c:v>557</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>615</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>788</c:v>
+                  <c:v>858</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>953</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1100</c:v>
+                  <c:v>1140</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1220</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1372</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1580</c:v>
+                  <c:v>1620</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1672</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1666</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1661</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1624</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1618</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1618</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1617</c:v>
+                  <c:v>1590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,7 +321,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6E8B-4AFF-9538-61891ADF8E7A}"/>
+              <c16:uniqueId val="{00000000-91D7-4868-8D69-F76BE5237716}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -694,10 +664,9 @@
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Hoja1!$B$3:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -730,7 +699,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v> </c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5.5</c:v>
@@ -738,8 +707,8 @@
                 <c:pt idx="12">
                   <c:v>6</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -748,43 +717,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>215</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>372</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>470</c:v>
+                  <c:v>557</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>615</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>788</c:v>
+                  <c:v>858</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>953</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1100</c:v>
+                  <c:v>1140</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1220</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1372</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1580</c:v>
+                  <c:v>1620</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1670</c:v>
+                  <c:v>1590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2099,16 +2068,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>669054</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>31608</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>71278</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>169556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>371929</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>536153</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:rowOff>38162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2135,16 +2104,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>670531</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>72755</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>184338</xdr:rowOff>
+      <xdr:rowOff>131786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>353786</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518010</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172358</xdr:rowOff>
+      <xdr:rowOff>119806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2489,407 +2458,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144CDF26-D914-4359-9B3B-99D0559A1B45}">
-  <dimension ref="B2:Q23"/>
+  <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="234" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2">
-        <v>1000</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>0.5</v>
-      </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-      <c r="M3">
-        <v>14000</v>
-      </c>
-      <c r="N3">
-        <f>$Q$3*(M3/(M3+$Q$2))</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="P3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1248</v>
+      </c>
+      <c r="E3">
+        <f>D3/2</f>
+        <v>624</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.6</v>
       </c>
       <c r="C4">
-        <v>70</v>
-      </c>
-      <c r="K4">
-        <v>0.7</v>
-      </c>
-      <c r="L4">
-        <v>42</v>
-      </c>
-      <c r="M4">
-        <v>5300</v>
-      </c>
-      <c r="N4">
-        <f>$Q$3*(M4/(M4+$Q$2))</f>
-        <v>4.2063492063492065</v>
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>10150</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="0">D4/2</f>
+        <v>5075</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>215</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>194</v>
-      </c>
-      <c r="M5">
-        <v>1830</v>
-      </c>
-      <c r="N5">
-        <f>$Q$3*(M5/(M5+$Q$2))</f>
-        <v>3.2332155477031805</v>
+        <v>237</v>
+      </c>
+      <c r="D5">
+        <v>21350</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>10675</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.5</v>
       </c>
       <c r="C6">
-        <v>372</v>
-      </c>
-      <c r="K6">
-        <v>1.5</v>
-      </c>
-      <c r="L6">
-        <v>331</v>
-      </c>
-      <c r="M6">
-        <v>1288</v>
-      </c>
-      <c r="N6">
-        <f>$Q$3*(M6/(M6+$Q$2))</f>
-        <v>2.8146853146853146</v>
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>24500</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>12250</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>470</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <v>460</v>
-      </c>
-      <c r="M7">
-        <v>1045</v>
-      </c>
-      <c r="N7">
-        <f>$Q$3*(M7/(M7+$Q$2))</f>
-        <v>2.5550122249388751</v>
+        <v>557</v>
+      </c>
+      <c r="D7">
+        <v>26230</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>13115</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2.5</v>
       </c>
       <c r="C8">
-        <v>615</v>
-      </c>
-      <c r="K8">
-        <v>2.5</v>
-      </c>
-      <c r="L8">
-        <v>583</v>
-      </c>
-      <c r="M8">
-        <v>901</v>
-      </c>
-      <c r="N8">
-        <f>$Q$3*(M8/(M8+$Q$2))</f>
-        <v>2.3698053655970543</v>
+        <v>712</v>
+      </c>
+      <c r="D8">
+        <v>27350</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>13675</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>788</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>721</v>
-      </c>
-      <c r="M9">
-        <v>789</v>
-      </c>
-      <c r="N9">
-        <f>$Q$3*(M9/(M9+$Q$2))</f>
-        <v>2.205142537730576</v>
+        <v>858</v>
+      </c>
+      <c r="D9">
+        <v>28200</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>14100</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>3.5</v>
       </c>
       <c r="C10">
-        <v>953</v>
-      </c>
-      <c r="K10">
-        <v>3.5</v>
-      </c>
-      <c r="L10">
-        <v>845</v>
-      </c>
-      <c r="M10">
-        <v>716</v>
-      </c>
-      <c r="N10">
-        <f>$Q$3*(M10/(M10+$Q$2))</f>
-        <v>2.0862470862470865</v>
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>28900</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>14450</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11">
-        <v>1100</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11">
-        <v>968</v>
-      </c>
-      <c r="M11">
-        <v>660</v>
-      </c>
-      <c r="N11">
-        <f>$Q$3*(M11/(M11+$Q$2))</f>
-        <v>1.9879518072289157</v>
+        <v>1140</v>
+      </c>
+      <c r="D11">
+        <v>29490</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>14745</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>4.5</v>
       </c>
       <c r="C12">
-        <v>1220</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
-      <c r="L12">
-        <v>1206</v>
-      </c>
-      <c r="M12">
-        <v>577</v>
-      </c>
-      <c r="N12">
-        <f>$Q$3*(M12/(M12+$Q$2))</f>
-        <v>1.829422954977806</v>
+        <v>1287</v>
+      </c>
+      <c r="D12">
+        <v>29960</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>14980</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>5</v>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>1372</v>
-      </c>
-      <c r="K13">
-        <v>6</v>
-      </c>
-      <c r="L13">
-        <v>1438</v>
-      </c>
-      <c r="M13">
-        <v>520</v>
-      </c>
-      <c r="N13">
-        <f>$Q$3*(M13/(M13+$Q$2))</f>
-        <v>1.7105263157894737</v>
+        <v>1297</v>
+      </c>
+      <c r="D13">
+        <v>29840</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>14920</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>5.5</v>
       </c>
       <c r="C14">
-        <v>1580</v>
-      </c>
-      <c r="K14">
-        <v>7</v>
-      </c>
-      <c r="L14">
-        <v>1630</v>
-      </c>
-      <c r="M14">
-        <v>485</v>
-      </c>
-      <c r="N14">
-        <f>$Q$3*(M14/(M14+$Q$2))</f>
-        <v>1.632996632996633</v>
+        <v>1620</v>
+      </c>
+      <c r="D14">
+        <v>30800</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>15400</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15">
-        <v>1670</v>
-      </c>
-      <c r="K15">
-        <v>8</v>
-      </c>
-      <c r="L15">
-        <v>1600</v>
-      </c>
-      <c r="M15">
-        <v>490</v>
-      </c>
-      <c r="N15">
-        <f>$Q$3*(M15/(M15+$Q$2))</f>
-        <v>1.644295302013423</v>
+        <v>1590</v>
+      </c>
+      <c r="D15">
+        <v>30800</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>15400</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>6.5</v>
       </c>
-      <c r="C16">
-        <v>1672</v>
-      </c>
-      <c r="K16">
-        <v>9</v>
-      </c>
-      <c r="L16">
-        <v>1570</v>
-      </c>
-      <c r="M16">
-        <v>493</v>
-      </c>
-      <c r="N16">
-        <f>$Q$3*(M16/(M16+$Q$2))</f>
-        <v>1.6510381781647689</v>
-      </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>7</v>
       </c>
-      <c r="C17">
-        <v>1670</v>
-      </c>
-      <c r="K17">
-        <v>10</v>
-      </c>
-      <c r="L17">
-        <v>1550</v>
-      </c>
-      <c r="M17">
-        <v>497</v>
-      </c>
-      <c r="N17">
-        <f>$Q$3*(M17/(M17+$Q$2))</f>
-        <v>1.6599866399465599</v>
-      </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>7.5</v>
       </c>
-      <c r="C18">
-        <v>1666</v>
-      </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>8</v>
       </c>
-      <c r="C19">
-        <v>1661</v>
-      </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>8.5</v>
       </c>
-      <c r="C20">
-        <v>1624</v>
-      </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>9</v>
       </c>
-      <c r="C21">
-        <v>1618</v>
-      </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>9.5</v>
       </c>
-      <c r="C22">
-        <v>1618</v>
-      </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>10</v>
-      </c>
-      <c r="C23">
-        <v>1617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>